<commit_message>
Updated Test Case and Report Structure
</commit_message>
<xml_diff>
--- a/avactisautomation/TestData/TestData.xlsx
+++ b/avactisautomation/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mubin\git\Avactis\avactisautomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60811CD0-CF0B-45D5-975D-92D4C730D2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574F65DA-6F4D-4948-9D20-A2B69AA2B478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,10 +55,10 @@
     <t>Takali Road</t>
   </si>
   <si>
-    <t>imapirjade1@gmail.com</t>
-  </si>
-  <si>
     <t>Mubin@1234</t>
+  </si>
+  <si>
+    <t>imapirjade116@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -422,9 +422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FBE3B7-95A1-49F3-A2E5-972BD8CE2554}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -440,7 +438,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -475,7 +473,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added changes for checkout of products
</commit_message>
<xml_diff>
--- a/avactisautomation/TestData/TestData.xlsx
+++ b/avactisautomation/TestData/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mubin\git\Avactis\avactisautomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574F65DA-6F4D-4948-9D20-A2B69AA2B478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8376E685-E231-41B4-80EE-EED5BC1BD13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="RegistrationDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="ProductList" sheetId="3" r:id="rId2"/>
+    <sheet name="RegistrationDetails" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>pirjademubinn@gmail.com</t>
   </si>
@@ -59,13 +60,28 @@
   </si>
   <si>
     <t>imapirjade116@gmail.com</t>
+  </si>
+  <si>
+    <t>PRODUCTS</t>
+  </si>
+  <si>
+    <t>Forbidden Planet</t>
+  </si>
+  <si>
+    <t>Asus Eee PC Touch</t>
+  </si>
+  <si>
+    <t>EKTORP Neckroll</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +97,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -90,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,16 +122,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -419,10 +462,61 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE688020-4E00-463E-9F98-2F6916324712}">
+  <dimension ref="B2:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FBE3B7-95A1-49F3-A2E5-972BD8CE2554}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Updated placeorder method and verify price methods
</commit_message>
<xml_diff>
--- a/avactisautomation/TestData/TestData.xlsx
+++ b/avactisautomation/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mubin\git\Avactis\avactisautomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F2B8F6-B5F0-4366-AA5A-3C8A1964A79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EBE7EB-FDC5-4A4F-8ECA-8CCB8EDF2589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>pirjademubinn@gmail.com</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t>mubinpirjade@gmail.com</t>
+  </si>
+  <si>
+    <t>NTStartEnd</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>$48.59</t>
+  </si>
+  <si>
+    <t>$499.99</t>
+  </si>
+  <si>
+    <t>$9.99</t>
   </si>
 </sst>
 </file>
@@ -467,48 +482,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE688020-4E00-463E-9F98-2F6916324712}">
-  <dimension ref="B2:C5"/>
+  <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -588,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D43C52-F79F-4B45-8AF5-CEBAEB9FD30A}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated methods from Admin Page
</commit_message>
<xml_diff>
--- a/avactisautomation/TestData/TestData.xlsx
+++ b/avactisautomation/TestData/TestData.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mubin\git\Avactis\avactisautomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EBE7EB-FDC5-4A4F-8ECA-8CCB8EDF2589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68031977-132B-4E35-9BD4-5D69851A7027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="ProductList" sheetId="3" r:id="rId2"/>
-    <sheet name="RegistrationDetails" sheetId="2" r:id="rId3"/>
-    <sheet name="BillingDetails" sheetId="4" r:id="rId4"/>
+    <sheet name="AdminLogin" sheetId="5" r:id="rId3"/>
+    <sheet name="RegistrationDetails" sheetId="2" r:id="rId4"/>
+    <sheet name="BillingDetails" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>pirjademubinn@gmail.com</t>
   </si>
@@ -454,7 +455,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE688020-4E00-463E-9F98-2F6916324712}">
   <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -553,6 +554,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA96E82-0FB6-4FC3-B9EB-9B0078B409AA}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{035C8F63-E308-41CD-B343-B2C40472BABB}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{775054B7-CC86-4130-B268-39763546A38C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FBE3B7-95A1-49F3-A2E5-972BD8CE2554}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -620,7 +652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D43C52-F79F-4B45-8AF5-CEBAEB9FD30A}">
   <dimension ref="A1:J1"/>
   <sheetViews>

</xml_diff>